<commit_message>
Update 게시글 파일 명세서 by Pang 2020_01_17.xlsx
</commit_message>
<xml_diff>
--- a/게시글 파일 명세서 by Pang 2020_01_17.xlsx
+++ b/게시글 파일 명세서 by Pang 2020_01_17.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlarh\Documents\GitHub\verbose-octo-guacamole\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89B9AE0-8F21-4594-9BAD-840F30D69A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="18315" windowHeight="8730"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="99">
   <si>
     <t xml:space="preserve">파일 명세서 </t>
   </si>
@@ -156,13 +162,246 @@
   </si>
   <si>
     <t>BoardModifyFormAction.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActionForward</t>
+  </si>
+  <si>
+    <t>path 즉 주소? 를 넘겨주고 받는 vo 패키지 내에 ActionForward.java로 forward 라는 객체를 만들고 게시글의 번호를 받아오며</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> svc 패키지 내에 BoardDetailService.java 로 조회수를 가져온다. 후에 조회수가 0보다 높다면 그대로 해당 게시물을 출력한다.</t>
+  </si>
+  <si>
+    <t>BoardModifyProAction.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 후에 svc 패키지 내에BoardModifyProService를 이용해 객체 boardModifyProService를 생성  boolean 타입의 변수 isRightUser를 선언. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">boardModifyProService.isArticleWriter 메소드에 게시글 번호와 게시글 비밀번호를 넘겨서 실행하여 결과를 담는다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 번호와 게시글에 대한 정보를 BoardBean 형태의 article이라는 이름으로 받아온다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 후에 if 문으로 메소드의 실행결과 비밀번호가 일치하지 않을 경우 접근을 막고  else 문의 일치할 경우에는 해당 게시글의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 번호와 제목 내용을 article 에 set해준 뒤 article 을 다시 boardModifyProService.modifyArticle메소드에 담아 결과를 boolean 타입의 isModifySuccess에 담아준다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그 후에 isModifySuccess의 결과에 따라서 수정실패를 출력하거나 ActionForward 의 객체 forward 에 게시글의 번호를 담은 path 를 set해준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardReplyFormAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardReplyProAction</t>
+  </si>
+  <si>
+    <t>ActionForward forward 객체를 생성. Nowpage 라는String 타입을 getparameter page 를 받아와서 선언</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">게시글의 번호도 받아온다. 후에 BoardBean 의 article 에 boardDetailService클래스의 getArticle(board_num) 으로 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">게시글을 가져온다. 그 후에 그 게시글을 article 에 request.setAttribute 해주고 page에 nowPage 를 마찬가지로 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setAttribute 해준다. 후에 forward.setPath("/qna_board_reply.jsp"); 를 실행하고 forward 를 return 해준다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActionForward forward = null; forward 선언 . Nowpage 를 page 를 넘겨받아서 선언 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>. BoardBean article = new BoardBean();  생성해주고 게시글 번호와 게시글 이름,비밀번호,제목,내용,Board_re_ref,lev,seq 를 article 에 set해준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  후에 boardReplyProservice를 통해서 article 을 이용한 메소드의 실행 결과를 isReplySuccess 라는 boolean타입의 변수에 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담고 그 결과에 따라 if 문으로 성공하면  forward.setPath 로 boardList를 넘겨주고 아닐 경우에는 답장실패 문구와 함께 막아준다. 그 후에 forward 를 리턴해준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardWriteProAction</t>
+  </si>
+  <si>
+    <t>null 값을 가진 ActionForward forward 와 BoardBean boardBean을 선언 String realFolder라는 변수"";로 선언</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> String saveFolder라는 변수 "/boardUpload"로 선언.  int fileSize=5*1024*1024; 로 fileSize 를 선언. 인터페이스 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ServletContext 로 context 선언하여 request.getServletContext(); 실행한다.(자세히모름..) 아까 realFolder 변수에 현재 context 의 저장된 폴더를 realpath 를 넣어준다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultipartRequest…..(잘모름)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardWriteProService boardWriteProService 객체 생성 후 boolean 형태의 isWriteSuccess에 게시글 등록에 대한 결과값을 가져와 넣는다.그 후 결과 출력 실패시 막고 등록실패 출력 성공시 게시글 목록으로 이동한다. Forward 를 리하고 마무리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardBean 객체 생성 후 게시글 이름, 비밀번호, 제목, 내용 을 multi로 getParameter 해온다 .File 도 set ..해준다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>controller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardFrontController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">String command=RequestURI.substring(contextPath.length()); 을 통해서 접속된 페이지의 주소 이름을 넣는다. 후에 if 문을 통해서 넘어온 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">페이지의 위치에 따라서 setPath 를 해주고 forward 에 excute를 실행. Forward 가 공백이 아닐 때 정상적으로 들어갔으므로 정해진 path 로 보낸다.  doGet 과 doPost 메소드로 각자 기능을 실행 </t>
+  </si>
+  <si>
+    <t>dao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">실질적인 실행 java 파일로 각 기능들의 dao 이다. 싱글톤 패턴으로 처음 유무만 판단해주고 . </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">글의 개수를 구하는 selectListCount메소드 , ("select count(*) from board");로 글의 개수를 구한다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ArrayList&lt;BoardBean&gt; 메소드로 "select * from board order by BOARD_RE_REF desc,BOARD_RE_SEQ asc limit ?,10"; 실행 . </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">BoardBean selectArticle 받아온 게시글번호를 받아와서 게시글을 출력. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insertArticle 메소드로 게시글 등록. insertReplyArticle 글 답변 등록. updateArticle 글수정. deleteArticle로 글 삭제 . updateReadCount로 조회수를 업데이트 해준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isArticleBoardWriter메소드를 통해 게시글 번호를 확인하여 일치할경우 Boolean 형태를 넘겨 글쓴이인지 확인시켜준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JdbcUtil</t>
+  </si>
+  <si>
+    <t>db의 연결과 닫는 것을 관리하는 java 파일..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>svc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDeleteProService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">isArticleWriter 메소드로 권한에 대하여 작성자가 맞는지 확인한다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>removeArticle 메소드로 dao의 delete 메소드를 실행 후 결과를 반환한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDetailService</t>
+  </si>
+  <si>
+    <t>게시물을 클릭했을 때 게시물을 자세히 보는 java 파일. 조회수를 증가시켜주는 메소드가 있고 dao 를 통해 select 하는 메소드가있다.  후에 article 을 반환한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardListService</t>
+  </si>
+  <si>
+    <t>getListCount 메소드로 게시글 개수를 세고 한페이지에 올릴 수 있는 최대 페이지를 정해서 그만큼만 출력해준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardReplyProService</t>
+  </si>
+  <si>
+    <t>게시글 답변을 담당하는 java 파일 답변게시글을 쓰고 그에 따른 결과를 반환.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardWriteProService</t>
+  </si>
+  <si>
+    <t>게시글을 입력하는 java 파일 게시글을 입력하여 그에 따른 결과를 반환.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardModifyProService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isArticleWriter메소드와 modifyArticle 로 게시글의 번호와 비번을 확인하여 맞으면 결과를 리턴.. 그 후에 수정 메소드로 수정 실행하여 결과를 다시 리턴 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardBean</t>
+  </si>
+  <si>
+    <t>PageInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isRedirect 과 path 겟터셋터.. 하는 dto </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">게시글에 대한 모든 정보들 dto </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이징을 담당하는 dto..</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -219,6 +458,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -266,7 +508,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,9 +541,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -334,6 +593,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,11 +785,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -702,19 +978,359 @@
       <c r="C23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+      <c r="D60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>37</v>
+      </c>
+      <c r="D69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D71" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>2</v>
       </c>
     </row>
@@ -726,7 +1342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -739,7 +1355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>